<commit_message>
propulsion test data scripts
</commit_message>
<xml_diff>
--- a/FFUAV Purchase Orders/tube_clampscrew_nylocknut_MCMASTER.xlsx
+++ b/FFUAV Purchase Orders/tube_clampscrew_nylocknut_MCMASTER.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://virginiatech-my.sharepoint.com/personal/jamesdrosdick_vt_edu/Documents/Documents/GitHub/Team_45_FFUAV/FFUAV Purchase Orders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{F8552153-4BE4-4825-85D6-01B8429EB794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAE48A00-E749-4EE9-AAC0-A69565F3E46E}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{F8552153-4BE4-4825-85D6-01B8429EB794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E1549D4-35C2-4747-8E17-8E50CF252CC1}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5100" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1572" yWindow="3744" windowWidth="21816" windowHeight="9768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplier 1" sheetId="1" r:id="rId1"/>
@@ -537,6 +537,45 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,15 +591,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -590,36 +620,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -919,8 +919,8 @@
   </sheetPr>
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="40" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,14 +947,14 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="49"/>
-      <c r="I3" s="53">
+      <c r="H3" s="33"/>
+      <c r="I3" s="30">
         <v>44952</v>
       </c>
-      <c r="J3" s="50"/>
+      <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -979,95 +979,95 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
       <c r="I6" s="10"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
       <c r="H8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="47">
         <v>117023</v>
       </c>
-      <c r="J8" s="34"/>
+      <c r="J8" s="47"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="48"/>
-      <c r="C9" s="35">
+      <c r="B9" s="32"/>
+      <c r="C9" s="39">
         <v>9198244073</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
-      <c r="H9" s="40" t="s">
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="H9" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="41"/>
-      <c r="J9" s="43"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="53"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="44"/>
-      <c r="J10" s="46"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="56"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="53" t="s">
+      <c r="I12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="50"/>
+      <c r="J12" s="31"/>
     </row>
     <row r="13" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-      <c r="I13" s="38" t="s">
+      <c r="C13" s="51"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="53"/>
+      <c r="I13" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="38"/>
+      <c r="J13" s="48"/>
       <c r="O13" s="13"/>
       <c r="S13">
         <f>7*30.38</f>
@@ -1075,21 +1075,21 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="44"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="56"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="37"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
       <c r="S15">
         <f>7*329.9</f>
         <v>2309.2999999999997</v>
@@ -1099,17 +1099,17 @@
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
     </row>
     <row r="18" spans="1:24" ht="7.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:24" ht="7.35" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1120,13 +1120,13 @@
       <c r="B20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1147,13 +1147,13 @@
       <c r="B21" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="57"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="38"/>
       <c r="H21" s="11" t="s">
         <v>29</v>
       </c>
@@ -1174,13 +1174,13 @@
       <c r="B22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
       <c r="H22" s="21" t="s">
         <v>46</v>
       </c>
@@ -1202,13 +1202,13 @@
       <c r="B23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="21" t="s">
         <v>45</v>
       </c>
@@ -1237,13 +1237,13 @@
       <c r="B24" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="23" t="s">
         <v>49</v>
       </c>
@@ -1261,11 +1261,11 @@
     <row r="25" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="25"/>
       <c r="I25" s="24"/>
       <c r="J25" s="5">
@@ -1277,11 +1277,11 @@
     <row r="26" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="52"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
       <c r="H26" s="25"/>
       <c r="I26" s="24"/>
       <c r="J26" s="5">
@@ -1293,11 +1293,11 @@
     <row r="27" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="52"/>
-      <c r="G27" s="52"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
       <c r="H27" s="25"/>
       <c r="I27" s="24"/>
       <c r="J27" s="5">
@@ -1309,11 +1309,11 @@
     <row r="28" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="52"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
       <c r="H28" s="25"/>
       <c r="I28" s="24"/>
       <c r="J28" s="5">
@@ -1325,11 +1325,11 @@
     <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="25"/>
       <c r="I29" s="24"/>
       <c r="J29" s="5">
@@ -1341,11 +1341,11 @@
     <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
       <c r="H30" s="25"/>
       <c r="I30" s="24"/>
       <c r="J30" s="5">
@@ -1357,11 +1357,11 @@
     <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
       <c r="H31" s="25"/>
       <c r="I31" s="24"/>
       <c r="J31" s="5">
@@ -1373,11 +1373,11 @@
     <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="20"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
       <c r="H32" s="25"/>
       <c r="I32" s="24"/>
       <c r="J32" s="5">
@@ -1389,11 +1389,11 @@
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
       <c r="H33" s="25"/>
       <c r="I33" s="24"/>
       <c r="J33" s="5">
@@ -1405,11 +1405,11 @@
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="20"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
       <c r="H34" s="25"/>
       <c r="I34" s="24"/>
       <c r="J34" s="5">
@@ -1419,27 +1419,27 @@
       <c r="K34" s="20"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H35" s="31" t="s">
+      <c r="H35" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="I35" s="31"/>
+      <c r="I35" s="44"/>
       <c r="J35" s="4">
         <f>SUM(J22:J34)</f>
         <v>115.75</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H36" s="32" t="s">
+      <c r="H36" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I36" s="32"/>
+      <c r="I36" s="45"/>
       <c r="J36" s="24"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="H37" s="33" t="s">
+      <c r="H37" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="I37" s="33"/>
+      <c r="I37" s="46"/>
       <c r="J37" s="3">
         <f>J36+J35</f>
         <v>115.75</v>
@@ -1453,28 +1453,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="C25:G25"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C33:G33"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
     <mergeCell ref="C34:G34"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="H36:I36"/>
@@ -1489,12 +1467,36 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="I9:J10"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" xr:uid="{87E8B9F7-BB4D-4AF2-89AE-F80F276D66BB}"/>
     <hyperlink ref="K24" r:id="rId2" xr:uid="{5EA4D7DD-47C0-4141-A064-01F582EDC3AA}"/>
+    <hyperlink ref="K22" r:id="rId3" xr:uid="{DEF8D0B7-FBA7-4560-9A99-6C071AE20E42}"/>
+    <hyperlink ref="K23" r:id="rId4" xr:uid="{829F2F9C-95FF-44F5-B759-094E76BE89BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="75" orientation="portrait" r:id="rId3"/>
+  <pageSetup scale="75" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>